<commit_message>
High score section added and a lot of functionality, bugs to work out still.
</commit_message>
<xml_diff>
--- a/Questions.xlsx
+++ b/Questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal\College\Continuing Education\UW Coding Bootcamp\Class-work-completed\04-Week\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08435D19-F2FF-48C1-90C4-7DAAEC6A8FFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9070540C-7957-498E-87E1-6C2040CFCF03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{33B19AFC-D07C-4861-A1A6-EF3E6EB70B58}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{33B19AFC-D07C-4861-A1A6-EF3E6EB70B58}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1254,18 +1254,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{734DF18D-FD0D-4310-9ED0-C45E8F8D3F07}">
   <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A29" sqref="A29:XFD29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="73.7109375" customWidth="1"/>
     <col min="3" max="3" width="17.5703125" customWidth="1"/>
-    <col min="4" max="4" width="30.28515625" customWidth="1"/>
-    <col min="5" max="5" width="37.42578125" customWidth="1"/>
-    <col min="6" max="6" width="26.28515625" customWidth="1"/>
+    <col min="4" max="4" width="60.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="49.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28.85546875" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>